<commit_message>
📝 Correct militancies of some people
</commit_message>
<xml_diff>
--- a/constituyentes/data/constituyentes.xlsx
+++ b/constituyentes/data/constituyentes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fguinez/Documents/Visualizaciones/quevotaron/constituyentes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8AA985-9CFC-3342-B676-A5D17B5CF8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75E96BA-D7A4-394B-9E74-CD0EB22DA96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="13360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constituyentes" sheetId="2" r:id="rId1"/>
+    <sheet name="resumen" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="237">
   <si>
     <t>Distrito/Pueblo</t>
   </si>
@@ -913,7 +914,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1093,8 +1094,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1220,6 +1233,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1265,12 +1307,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1316,7 +1362,490 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1839,36 +2368,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Constituyentes" displayName="Constituyentes" ref="A1:N157" totalsRowCount="1" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Constituyentes" displayName="Constituyentes" ref="A1:N157" totalsRowCount="1" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A1:N156" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:N156">
     <sortCondition ref="B1:B156"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nombre" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="12"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Militancia" totalsRowFunction="custom" dataDxfId="24" totalsRowDxfId="11">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nombre" totalsRowFunction="count" dataDxfId="42" totalsRowDxfId="29"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Militancia" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="28">
       <totalsRowFormula array="1">SUMPRODUCT(1/COUNTIF(Constituyentes[Militancia],Constituyentes[Militancia]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Militancia 2" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="10">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Militancia 2" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="27">
       <totalsRowFormula array="1">SUMPRODUCT(1/COUNTIF(Constituyentes[Militancia 2],Constituyentes[Militancia 2]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Coalición" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="9">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Coalición" totalsRowFunction="custom" dataDxfId="39" totalsRowDxfId="26">
       <totalsRowFormula array="1">SUMPRODUCT(1/COUNTIF(Constituyentes[Coalición],Constituyentes[Coalición]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Vocería de los Pueblos" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Subpacto" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="7">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Vocería de los Pueblos" totalsRowFunction="count" dataDxfId="38" totalsRowDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Subpacto" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="24">
       <totalsRowFormula array="1">SUMPRODUCT(1/COUNTIF(Constituyentes[Subpacto],Constituyentes[Subpacto]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Pacto" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="6">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Pacto" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="23">
       <totalsRowFormula array="1">SUMPRODUCT(1/COUNTIF(Constituyentes[Pacto],Constituyentes[Pacto]))</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="G" dataDxfId="18" totalsRowDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Votos Lista/Zona" dataDxfId="17" totalsRowDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Votos Constituyente" dataDxfId="16" totalsRowDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="% Lista" dataDxfId="15" totalsRowDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="% Constituyente" dataDxfId="14" totalsRowDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Distrito/Pueblo" dataDxfId="13" totalsRowDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="G" dataDxfId="35" totalsRowDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Votos Lista/Zona" dataDxfId="34" totalsRowDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Votos Constituyente" dataDxfId="33" totalsRowDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="% Lista" dataDxfId="32" totalsRowDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="% Constituyente" dataDxfId="31" totalsRowDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Distrito/Pueblo" dataDxfId="30" totalsRowDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E209196-D75E-1C4A-8A11-73FF39088169}" name="Tabla1" displayName="Tabla1" ref="A1:F156" headerRowDxfId="6" dataDxfId="7" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:F156" xr:uid="{E50B5797-F60B-F743-89CD-741801BBEE5F}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{F967CB53-3E67-1B47-9C8B-C88C0418F57F}" name="ID" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{7FD862BA-D954-6C47-86FA-8A70D489D225}" name="Nombre" dataDxfId="12" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{AE736CE6-3784-CD4A-996D-C5A712309EA1}" name="G" dataDxfId="11" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{9CEADDE8-371F-4C42-AA85-42745D5BDC9C}" name="Militancia" dataDxfId="10" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{58D81758-C4B4-4B46-A97E-F8F7C026707A}" name="Coalición" dataDxfId="9" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{9B93C7AB-E834-AF43-BB88-BE8B287254E1}" name="Vocería de los Pueblos" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2173,8 +2717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2331,7 +2875,7 @@
         <v>216</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>221</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>214</v>
@@ -2448,7 +2992,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>96</v>
@@ -2492,7 +3036,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -2536,7 +3080,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>140</v>
@@ -2664,7 +3208,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>60</v>
@@ -2834,7 +3378,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>161</v>
@@ -2878,7 +3422,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>182</v>
@@ -3090,7 +3634,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>136</v>
@@ -3176,7 +3720,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>30</v>
@@ -3220,7 +3764,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>173</v>
@@ -3348,7 +3892,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>19</v>
@@ -3527,7 +4071,7 @@
         <v>216</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>18</v>
+        <v>221</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>214</v>
@@ -3602,7 +4146,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>15</v>
@@ -3646,7 +4190,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>132</v>
@@ -3858,7 +4402,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>27</v>
@@ -3902,7 +4446,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>124</v>
@@ -4030,7 +4574,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>138</v>
+        <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>102</v>
@@ -4074,7 +4618,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>145</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>200</v>
@@ -4536,7 +5080,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>170</v>
@@ -4916,7 +5460,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>152</v>
+        <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>235</v>
@@ -5042,7 +5586,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>147</v>
+        <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>236</v>
@@ -5084,7 +5628,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>74</v>
@@ -5128,7 +5672,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>155</v>
+        <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>119</v>
@@ -5296,7 +5840,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>73</v>
@@ -5466,7 +6010,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>155</v>
@@ -5594,7 +6138,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>150</v>
@@ -6018,7 +6562,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>62</v>
@@ -6104,7 +6648,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>151</v>
+        <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>115</v>
@@ -6146,7 +6690,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>148</v>
+        <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>111</v>
@@ -6188,7 +6732,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>25</v>
@@ -6400,7 +6944,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>34</v>
@@ -6738,7 +7282,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>31</v>
@@ -6866,7 +7410,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>158</v>
@@ -7330,7 +7874,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>202</v>
@@ -7750,7 +8294,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>55</v>
+        <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>145</v>
@@ -8046,7 +8590,7 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>88</v>
@@ -8132,7 +8676,7 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>44</v>
@@ -8216,7 +8760,7 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>169</v>
@@ -8344,7 +8888,7 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>138</v>
@@ -8428,7 +8972,7 @@
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>141</v>
@@ -8472,7 +9016,7 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>198</v>
@@ -8516,7 +9060,7 @@
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>63</v>
@@ -8600,7 +9144,7 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
         <v>105</v>
@@ -8644,7 +9188,7 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>34</v>
+        <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
         <v>40</v>
@@ -8768,7 +9312,7 @@
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>81</v>
@@ -8821,7 +9365,7 @@
       </c>
       <c r="D157" s="2" cm="1">
         <f t="array" ref="D157">SUMPRODUCT(1/COUNTIF(Constituyentes[Militancia 2],Constituyentes[Militancia 2]))</f>
-        <v>17.999999999999986</v>
+        <v>17.999999999999982</v>
       </c>
       <c r="E157" s="2" cm="1">
         <f t="array" ref="E157">SUMPRODUCT(1/COUNTIF(Constituyentes[Coalición],Constituyentes[Coalición]))</f>
@@ -8850,6 +9394,2926 @@
       <c r="E158">
         <f>SUBTOTAL(103,Constituyentes[Coalición])</f>
         <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9DB618-C509-D242-9FDA-BFF3D1B5F105}">
+  <dimension ref="A1:F156"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>48</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>50</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F56" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>56</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>58</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>60</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>64</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F65" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F68" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>68</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F69" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F70" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>70</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>72</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F74" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>74</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F76" s="5"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>76</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F78" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>78</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>80</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F81" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>82</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F84" s="5"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>84</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F86" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>86</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F88" s="5"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <v>90</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F91" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>92</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F93" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F94" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <v>94</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F95" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>96</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F97" s="6"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>98</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F99" s="6"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F100" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>100</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F101" s="6"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="5">
+        <v>101</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F102" s="5"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="6">
+        <v>102</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F103" s="6"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="5">
+        <v>103</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F104" s="5"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="6">
+        <v>104</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F105" s="6"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="5">
+        <v>105</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F106" s="5"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="6">
+        <v>106</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F107" s="6"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="5">
+        <v>107</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F108" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="6">
+        <v>108</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F109" s="6"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="5">
+        <v>109</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F110" s="5"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="6">
+        <v>110</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F111" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="5">
+        <v>111</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F112" s="5"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="6">
+        <v>112</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F113" s="6"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="5">
+        <v>113</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F114" s="5"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="6">
+        <v>114</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F115" s="6"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="5">
+        <v>115</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F116" s="5"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="6">
+        <v>116</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F117" s="6"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="5">
+        <v>117</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F118" s="5"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="6">
+        <v>118</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F119" s="6"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="5">
+        <v>119</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F120" s="5"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="6">
+        <v>120</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F121" s="6"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="5">
+        <v>121</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F122" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="6">
+        <v>122</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F123" s="6"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="5">
+        <v>123</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F124" s="5"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="6">
+        <v>124</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F125" s="6"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="5">
+        <v>125</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C126" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F126" s="5"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="6">
+        <v>126</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F127" s="6"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="5">
+        <v>127</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F128" s="5"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="6">
+        <v>128</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F129" s="6"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="5">
+        <v>129</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F130" s="5"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="6">
+        <v>130</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F131" s="6"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="5">
+        <v>131</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C132" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F132" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="6">
+        <v>132</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F133" s="6"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="5">
+        <v>133</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F134" s="5"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="6">
+        <v>134</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F135" s="6"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="5">
+        <v>135</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F136" s="5"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="6">
+        <v>136</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F137" s="6"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="5">
+        <v>137</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="F138" s="5"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="6">
+        <v>138</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F139" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="5">
+        <v>139</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F140" s="5"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="6">
+        <v>140</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F141" s="6"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="5">
+        <v>141</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F142" s="5"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="6">
+        <v>142</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C143" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D143" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F143" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="5">
+        <v>143</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F144" s="5"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="6">
+        <v>144</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C145" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F145" s="6"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="5">
+        <v>145</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F146" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="6">
+        <v>146</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D147" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F147" s="6"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="5">
+        <v>147</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D148" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F148" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="6">
+        <v>148</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D149" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F149" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="5">
+        <v>149</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D150" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F150" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="6">
+        <v>150</v>
+      </c>
+      <c r="B151" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C151" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F151" s="6"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="5">
+        <v>151</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D152" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E152" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F152" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="6">
+        <v>152</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C153" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F153" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="5">
+        <v>153</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C154" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E154" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F154" s="5"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="6">
+        <v>154</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C155" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D155" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F155" s="6"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="8">
+        <v>155</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E156" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F156" s="8">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>